<commit_message>
create r codes for data presentation standards
</commit_message>
<xml_diff>
--- a/docs/test_svy_stat_funs.xlsx
+++ b/docs/test_svy_stat_funs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ligongc\Desktop\nhanes-shiny-bp\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5C76E729-5742-433F-9C69-E63A953B9A2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8DBACA0-BEAC-4557-8B09-C94B40A70E68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{FADFFF94-5C62-45D9-9C7A-10947175B043}"/>
   </bookViews>
@@ -967,7 +967,7 @@
   <dimension ref="B1:H11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
+      <selection activeCell="E2" sqref="E2:E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1243,8 +1243,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{091EB520-C6F5-43FC-9167-5100308459C4}">
   <dimension ref="B1:U11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>